<commit_message>
Completed the Comand Table; haven't checked it with the Professor or with the program.
</commit_message>
<xml_diff>
--- a/Commands Table.xlsx
+++ b/Commands Table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>ALUOp</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
   </si>
   <si>
     <t>MemWrite</t>
@@ -338,7 +350,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -377,15 +389,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -501,10 +504,10 @@
     <row r="13">
       <c r="B13" s="4"/>
       <c r="C13" t="s" s="4">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -836,15 +839,33 @@
       <c r="A3" t="s" s="12">
         <v>42</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="22" customHeight="1">
       <c r="A4" t="s" s="12">
@@ -868,9 +889,15 @@
       <c r="G4" s="14">
         <v>1</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" ht="22" customHeight="1">
       <c r="A5" t="s" s="12">
@@ -889,14 +916,20 @@
         <v>0</v>
       </c>
       <c r="F5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" ht="22" customHeight="1">
       <c r="A6" t="s" s="12">
@@ -915,14 +948,20 @@
         <v>0</v>
       </c>
       <c r="F6" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="14">
         <v>2</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" ht="22" customHeight="1">
       <c r="A7" t="s" s="12">
@@ -931,20 +970,34 @@
       <c r="B7" s="13">
         <v>111</v>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
+      <c r="C7" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="F7" s="14">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s" s="14">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s" s="14">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s" s="14">
+        <v>50</v>
+      </c>
+      <c r="J7" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" ht="22" customHeight="1">
       <c r="A8" t="s" s="12">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B8" s="13">
         <v>0</v>
@@ -964,13 +1017,19 @@
       <c r="G8" s="14">
         <v>0</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" ht="22" customHeight="1">
       <c r="A9" t="s" s="12">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B9" s="13">
         <v>0</v>
@@ -988,15 +1047,21 @@
         <v>1</v>
       </c>
       <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+      <c r="J9" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" t="s" s="12">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
@@ -1016,40 +1081,46 @@
       <c r="G10" s="14">
         <v>0</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" t="s" s="12">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s" s="19">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s" s="19">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s" s="19">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s" s="19">
         <v>54</v>
       </c>
-      <c r="F11" t="s" s="19">
+      <c r="B11" t="s" s="16">
         <v>55</v>
       </c>
-      <c r="G11" t="s" s="19">
+      <c r="C11" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="H11" t="s" s="19">
+      <c r="D11" t="s" s="16">
         <v>57</v>
       </c>
-      <c r="I11" t="s" s="19">
-        <v>57</v>
-      </c>
-      <c r="J11" t="s" s="19">
+      <c r="E11" t="s" s="16">
         <v>58</v>
+      </c>
+      <c r="F11" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s" s="16">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s" s="16">
+        <v>61</v>
+      </c>
+      <c r="I11" t="s" s="16">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s" s="16">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1072,28 +1143,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.2188" style="20" customWidth="1"/>
-    <col min="2" max="2" width="15.2188" style="20" customWidth="1"/>
-    <col min="3" max="3" width="15.2188" style="20" customWidth="1"/>
-    <col min="4" max="256" width="12.25" style="20" customWidth="1"/>
+    <col min="1" max="1" width="15.2188" style="17" customWidth="1"/>
+    <col min="2" max="2" width="15.2188" style="17" customWidth="1"/>
+    <col min="3" max="3" width="15.2188" style="17" customWidth="1"/>
+    <col min="4" max="256" width="12.25" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="21">
-        <v>59</v>
+      <c r="A1" t="s" s="18">
+        <v>63</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
     </row>
     <row r="2" ht="21" customHeight="1">
-      <c r="A2" t="s" s="22">
+      <c r="A2" t="s" s="19">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="23">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>62</v>
+      <c r="B2" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s" s="21">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>